<commit_message>
Migrate to V8 Add new nodo WOE
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/16_Inst_Properties_Predictive.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/16_Inst_Properties_Predictive.xlsx
@@ -136,7 +136,7 @@
     <t>DataFieldMatrixFormula</t>
   </si>
   <si>
-    <t>LIB_ISP.getDataFieldListForMatrix</t>
+    <t>LIB_EW.getDataFieldListForMatrix</t>
   </si>
 </sst>
 </file>
@@ -490,6 +490,54 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="12544425" cy="9715500"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13963650" cy="9915525"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -782,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +858,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>